<commit_message>
Fixed issue with the staff edit spinner value checks
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/User/ManagerData.xlsx
+++ b/Group14-A2/src/main/java/User/ManagerData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\javafx-restaurant-app\Group14-A2\src\main\java\User\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\User\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250C73D7-8D01-4180-ABDD-8DCE46F1C0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027C2FC3-FEC4-45BC-A0E0-483DA1667D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Data" sheetId="1" r:id="rId1"/>
@@ -124,9 +124,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -164,7 +164,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -270,7 +270,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -412,7 +412,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -423,22 +423,22 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.54296875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5546875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.453125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.54296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.0" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.0" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.36328125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.5546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +467,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -487,7 +487,7 @@
         <v>10</v>
       </c>
       <c r="G2" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
       <c r="H2" t="n">
         <v>28.0</v>
@@ -496,7 +496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6</v>
       </c>

</xml_diff>